<commit_message>
08/28/24 - Added Annual Augmented Payout Ratio
I added a field to the calculator control panel called "Annual Augmented Payout Ratio". This was added to both versions: Web and Excel.

This allows firms to be better valued. Many firms return much of the equity to shareholders through buybacks or dividends. I did not account for these returns of capital. Instead, all capital was previously assumed to remain in the business and accumulate in equity. This caused residual income values for each year (and predicted stock price) to be lower.

If net income is positive, a portion of net income is spent on buybacks or dividends each year (augmented payout ratio). Next year's book value only increases by the amount of net income that is leftover after dividends or buybacks.

If net income is negative, buybacks and dividends are assumed to not occur (since the firm is unprofitable). The entire loss is subtracted from book value to get next year's book value.
</commit_message>
<xml_diff>
--- a/Residual Income Valuation.xlsx
+++ b/Residual Income Valuation.xlsx
@@ -2,8 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA919C4-D68C-4086-AD1F-2043AFE38647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Diego\Entertainment\Technology Hobbies\ValueVille\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B9B299-C849-4A09-99C0-84F6A1318EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{1F977004-A12D-47CA-BAC2-9D34EBC4AB6C}"/>
   </bookViews>
@@ -52,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>($ in millions)</t>
   </si>
@@ -121,6 +126,9 @@
   </si>
   <si>
     <t>Effective Tax Rate</t>
+  </si>
+  <si>
+    <t>Annual Augmented Payout Ratio</t>
   </si>
 </sst>
 </file>
@@ -564,7 +572,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -694,34 +702,35 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="169" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="22" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="19" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="22" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="20" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="17" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="17" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="14" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="14" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="21" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Bad" xfId="3" builtinId="27" customBuiltin="1"/>
@@ -1028,10 +1037,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFDFE9F4"/>
   </sheetPr>
-  <dimension ref="A3:U54"/>
+  <dimension ref="A3:U55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="13.15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1130,46 +1139,46 @@
       <c r="B6" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="84">
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="89">
         <v>1000</v>
       </c>
-      <c r="H6" s="85" cm="1">
+      <c r="H6" s="90" cm="1">
         <f t="array" ref="H6">bankers_round(G6*(1+H7), 2)</f>
         <v>1100</v>
       </c>
-      <c r="I6" s="85" cm="1">
+      <c r="I6" s="90" cm="1">
         <f t="array" ref="I6">bankers_round(H6*(1+I7), 2)</f>
         <v>1210</v>
       </c>
-      <c r="J6" s="85" cm="1">
+      <c r="J6" s="90" cm="1">
         <f t="array" ref="J6">bankers_round(I6*(1+J7), 2)</f>
         <v>1331</v>
       </c>
-      <c r="K6" s="85" cm="1">
+      <c r="K6" s="90" cm="1">
         <f t="array" ref="K6">bankers_round(J6*(1+K7), 2)</f>
         <v>1464.1</v>
       </c>
-      <c r="L6" s="85" cm="1">
+      <c r="L6" s="90" cm="1">
         <f t="array" ref="L6">bankers_round(K6*(1+L7), 2)</f>
         <v>1610.51</v>
       </c>
-      <c r="M6" s="85" cm="1">
+      <c r="M6" s="90" cm="1">
         <f t="array" ref="M6">bankers_round(L6*(1+M7), 2)</f>
         <v>1771.56</v>
       </c>
-      <c r="N6" s="85" cm="1">
+      <c r="N6" s="90" cm="1">
         <f t="array" ref="N6">bankers_round(M6*(1+N7), 2)</f>
         <v>1948.72</v>
       </c>
-      <c r="O6" s="85" cm="1">
+      <c r="O6" s="90" cm="1">
         <f t="array" ref="O6">bankers_round(N6*(1+O7), 2)</f>
         <v>2143.59</v>
       </c>
-      <c r="P6" s="85" cm="1">
+      <c r="P6" s="90" cm="1">
         <f t="array" ref="P6">bankers_round(O6*(1+P7), 2)</f>
         <v>2357.9499999999998</v>
       </c>
@@ -1182,36 +1191,36 @@
       <c r="B7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="89"/>
-      <c r="H7" s="90">
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="93">
         <v>0.1</v>
       </c>
-      <c r="I7" s="90">
+      <c r="I7" s="93">
         <v>0.1</v>
       </c>
-      <c r="J7" s="90">
+      <c r="J7" s="93">
         <v>0.1</v>
       </c>
-      <c r="K7" s="90">
+      <c r="K7" s="93">
         <v>0.1</v>
       </c>
-      <c r="L7" s="90">
+      <c r="L7" s="93">
         <v>0.1</v>
       </c>
-      <c r="M7" s="90">
+      <c r="M7" s="93">
         <v>0.1</v>
       </c>
-      <c r="N7" s="90">
+      <c r="N7" s="93">
         <v>0.1</v>
       </c>
-      <c r="O7" s="90">
+      <c r="O7" s="93">
         <v>0.1</v>
       </c>
-      <c r="P7" s="90">
+      <c r="P7" s="93">
         <v>0.1</v>
       </c>
       <c r="Q7" s="67">
@@ -1222,36 +1231,36 @@
       <c r="B8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="91">
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="84">
         <v>0.5</v>
       </c>
-      <c r="I8" s="91">
+      <c r="I8" s="84">
         <v>0.5</v>
       </c>
-      <c r="J8" s="91">
+      <c r="J8" s="84">
         <v>0.5</v>
       </c>
-      <c r="K8" s="91">
+      <c r="K8" s="84">
         <v>0.5</v>
       </c>
-      <c r="L8" s="91">
+      <c r="L8" s="84">
         <v>0.5</v>
       </c>
-      <c r="M8" s="91">
+      <c r="M8" s="84">
         <v>0.5</v>
       </c>
-      <c r="N8" s="91">
+      <c r="N8" s="84">
         <v>0.5</v>
       </c>
-      <c r="O8" s="91">
+      <c r="O8" s="84">
         <v>0.5</v>
       </c>
-      <c r="P8" s="91">
+      <c r="P8" s="84">
         <v>0.5</v>
       </c>
       <c r="Q8" s="68">
@@ -1262,36 +1271,36 @@
       <c r="B9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="92">
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="94">
         <v>500</v>
       </c>
-      <c r="I9" s="92">
+      <c r="I9" s="94">
         <v>500</v>
       </c>
-      <c r="J9" s="92">
+      <c r="J9" s="94">
         <v>500</v>
       </c>
-      <c r="K9" s="92">
+      <c r="K9" s="94">
         <v>500</v>
       </c>
-      <c r="L9" s="92">
+      <c r="L9" s="94">
         <v>500</v>
       </c>
-      <c r="M9" s="92">
+      <c r="M9" s="94">
         <v>500</v>
       </c>
-      <c r="N9" s="92">
+      <c r="N9" s="94">
         <v>500</v>
       </c>
-      <c r="O9" s="92">
+      <c r="O9" s="94">
         <v>500</v>
       </c>
-      <c r="P9" s="92">
+      <c r="P9" s="94">
         <v>500</v>
       </c>
       <c r="Q9" s="69">
@@ -1302,36 +1311,36 @@
       <c r="B10" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="92">
-        <v>0</v>
-      </c>
-      <c r="I10" s="92">
-        <v>0</v>
-      </c>
-      <c r="J10" s="92">
-        <v>0</v>
-      </c>
-      <c r="K10" s="92">
-        <v>0</v>
-      </c>
-      <c r="L10" s="92">
-        <v>0</v>
-      </c>
-      <c r="M10" s="92">
-        <v>0</v>
-      </c>
-      <c r="N10" s="92">
-        <v>0</v>
-      </c>
-      <c r="O10" s="92">
-        <v>0</v>
-      </c>
-      <c r="P10" s="92">
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="92"/>
+      <c r="H10" s="94">
+        <v>0</v>
+      </c>
+      <c r="I10" s="94">
+        <v>0</v>
+      </c>
+      <c r="J10" s="94">
+        <v>0</v>
+      </c>
+      <c r="K10" s="94">
+        <v>0</v>
+      </c>
+      <c r="L10" s="94">
+        <v>0</v>
+      </c>
+      <c r="M10" s="94">
+        <v>0</v>
+      </c>
+      <c r="N10" s="94">
+        <v>0</v>
+      </c>
+      <c r="O10" s="94">
+        <v>0</v>
+      </c>
+      <c r="P10" s="94">
         <v>0</v>
       </c>
       <c r="Q10" s="69">
@@ -1342,36 +1351,36 @@
       <c r="B11" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="92">
-        <v>0</v>
-      </c>
-      <c r="I11" s="92">
-        <v>0</v>
-      </c>
-      <c r="J11" s="92">
-        <v>0</v>
-      </c>
-      <c r="K11" s="92">
-        <v>0</v>
-      </c>
-      <c r="L11" s="92">
-        <v>0</v>
-      </c>
-      <c r="M11" s="92">
-        <v>0</v>
-      </c>
-      <c r="N11" s="92">
-        <v>0</v>
-      </c>
-      <c r="O11" s="92">
-        <v>0</v>
-      </c>
-      <c r="P11" s="92">
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="94">
+        <v>0</v>
+      </c>
+      <c r="I11" s="94">
+        <v>0</v>
+      </c>
+      <c r="J11" s="94">
+        <v>0</v>
+      </c>
+      <c r="K11" s="94">
+        <v>0</v>
+      </c>
+      <c r="L11" s="94">
+        <v>0</v>
+      </c>
+      <c r="M11" s="94">
+        <v>0</v>
+      </c>
+      <c r="N11" s="94">
+        <v>0</v>
+      </c>
+      <c r="O11" s="94">
+        <v>0</v>
+      </c>
+      <c r="P11" s="94">
         <v>0</v>
       </c>
       <c r="Q11" s="69">
@@ -1389,45 +1398,45 @@
       <c r="G12" s="70">
         <v>500</v>
       </c>
-      <c r="H12" s="62" t="e" cm="1">
-        <f t="array" aca="1" ref="H12" ca="1">bankers_round((H6*H8-SUM(H9:H11))*(1-$G$18), 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I12" s="62" t="e" cm="1">
-        <f t="array" aca="1" ref="I12" ca="1">bankers_round((I6*I8-SUM(I9:I11))*(1-$G$18), 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J12" s="62" t="e" cm="1">
-        <f t="array" aca="1" ref="J12" ca="1">bankers_round((J6*J8-SUM(J9:J11))*(1-$G$18), 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K12" s="62" t="e" cm="1">
-        <f t="array" aca="1" ref="K12" ca="1">bankers_round((K6*K8-SUM(K9:K11))*(1-$G$18), 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L12" s="62" t="e" cm="1">
-        <f t="array" aca="1" ref="L12" ca="1">bankers_round((L6*L8-SUM(L9:L11))*(1-$G$18), 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M12" s="62" t="e" cm="1">
-        <f t="array" aca="1" ref="M12" ca="1">bankers_round((M6*M8-SUM(M9:M11))*(1-$G$18), 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N12" s="62" t="e" cm="1">
-        <f t="array" aca="1" ref="N12" ca="1">bankers_round((N6*N8-SUM(N9:N11))*(1-$G$18), 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="O12" s="62" t="e" cm="1">
-        <f t="array" aca="1" ref="O12" ca="1">bankers_round((O6*O8-SUM(O9:O11))*(1-$G$18), 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="P12" s="62" t="e" cm="1">
-        <f t="array" aca="1" ref="P12" ca="1">bankers_round((P6*P8-SUM(P9:P11))*(1-$G$18), 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Q12" s="63" t="e" cm="1">
-        <f t="array" aca="1" ref="Q12" ca="1">bankers_round((Q6*Q8-SUM(Q9:Q11))*(1-$G$18), 2)</f>
-        <v>#NAME?</v>
+      <c r="H12" s="62" cm="1">
+        <f t="array" ref="H12">bankers_round((H6*H8-SUM(H9:H11))*(1-$G$18), 2)</f>
+        <v>40.5</v>
+      </c>
+      <c r="I12" s="62" cm="1">
+        <f t="array" ref="I12">bankers_round((I6*I8-SUM(I9:I11))*(1-$G$18), 2)</f>
+        <v>85.05</v>
+      </c>
+      <c r="J12" s="62" cm="1">
+        <f t="array" ref="J12">bankers_round((J6*J8-SUM(J9:J11))*(1-$G$18), 2)</f>
+        <v>134.06</v>
+      </c>
+      <c r="K12" s="62" cm="1">
+        <f t="array" ref="K12">bankers_round((K6*K8-SUM(K9:K11))*(1-$G$18), 2)</f>
+        <v>187.96</v>
+      </c>
+      <c r="L12" s="62" cm="1">
+        <f t="array" ref="L12">bankers_round((L6*L8-SUM(L9:L11))*(1-$G$18), 2)</f>
+        <v>247.26</v>
+      </c>
+      <c r="M12" s="62" cm="1">
+        <f t="array" ref="M12">bankers_round((M6*M8-SUM(M9:M11))*(1-$G$18), 2)</f>
+        <v>312.48</v>
+      </c>
+      <c r="N12" s="62" cm="1">
+        <f t="array" ref="N12">bankers_round((N6*N8-SUM(N9:N11))*(1-$G$18), 2)</f>
+        <v>384.23</v>
+      </c>
+      <c r="O12" s="62" cm="1">
+        <f t="array" ref="O12">bankers_round((O6*O8-SUM(O9:O11))*(1-$G$18), 2)</f>
+        <v>463.15</v>
+      </c>
+      <c r="P12" s="62" cm="1">
+        <f t="array" ref="P12">bankers_round((P6*P8-SUM(P9:P11))*(1-$G$18), 2)</f>
+        <v>549.97</v>
+      </c>
+      <c r="Q12" s="63" cm="1">
+        <f t="array" ref="Q12">bankers_round((Q6*Q8-SUM(Q9:Q11))*(1-$G$18), 2)</f>
+        <v>645.46</v>
       </c>
       <c r="U12" s="72"/>
     </row>
@@ -1435,52 +1444,52 @@
       <c r="B13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="94"/>
-      <c r="G13" s="95">
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="97">
         <v>1000</v>
       </c>
-      <c r="H13" s="96" cm="1">
-        <f t="array" ref="H13">bankers_round(G13+G12, 2)</f>
+      <c r="H13" s="98" cm="1">
+        <f t="array" ref="H13">IF(H12&gt;0,bankers_round(G13+G12*(1-$G$21),2),bankers_round(G13+G12,2))</f>
         <v>1500</v>
       </c>
-      <c r="I13" s="96" t="e" cm="1">
-        <f t="array" aca="1" ref="I13" ca="1">bankers_round(H13+H12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J13" s="96" t="e" cm="1">
-        <f t="array" aca="1" ref="J13" ca="1">bankers_round(I13+I12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K13" s="96" t="e" cm="1">
-        <f t="array" aca="1" ref="K13" ca="1">bankers_round(J13+J12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L13" s="96" t="e" cm="1">
-        <f t="array" aca="1" ref="L13" ca="1">bankers_round(K13+K12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M13" s="96" t="e" cm="1">
-        <f t="array" aca="1" ref="M13" ca="1">bankers_round(L13+L12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N13" s="96" t="e" cm="1">
-        <f t="array" aca="1" ref="N13" ca="1">bankers_round(M13+M12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="O13" s="96" t="e" cm="1">
-        <f t="array" aca="1" ref="O13" ca="1">bankers_round(N13+N12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="P13" s="96" t="e" cm="1">
-        <f t="array" aca="1" ref="P13" ca="1">bankers_round(O13+O12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Q13" s="40" t="e" cm="1">
-        <f t="array" aca="1" ref="Q13" ca="1">bankers_round(P13+P12, 2)</f>
-        <v>#NAME?</v>
+      <c r="I13" s="98" cm="1">
+        <f t="array" ref="I13">IF(I12&gt;0,bankers_round(H13+H12*(1-$G$21),2),bankers_round(H13+H12,2))</f>
+        <v>1540.5</v>
+      </c>
+      <c r="J13" s="98" cm="1">
+        <f t="array" ref="J13">IF(J12&gt;0,bankers_round(I13+I12*(1-$G$21),2),bankers_round(I13+I12,2))</f>
+        <v>1625.55</v>
+      </c>
+      <c r="K13" s="98" cm="1">
+        <f t="array" ref="K13">IF(K12&gt;0,bankers_round(J13+J12*(1-$G$21),2),bankers_round(J13+J12,2))</f>
+        <v>1759.61</v>
+      </c>
+      <c r="L13" s="98" cm="1">
+        <f t="array" ref="L13">IF(L12&gt;0,bankers_round(K13+K12*(1-$G$21),2),bankers_round(K13+K12,2))</f>
+        <v>1947.57</v>
+      </c>
+      <c r="M13" s="98" cm="1">
+        <f t="array" ref="M13">IF(M12&gt;0,bankers_round(L13+L12*(1-$G$21),2),bankers_round(L13+L12,2))</f>
+        <v>2194.83</v>
+      </c>
+      <c r="N13" s="98" cm="1">
+        <f t="array" ref="N13">IF(N12&gt;0,bankers_round(M13+M12*(1-$G$21),2),bankers_round(M13+M12,2))</f>
+        <v>2507.31</v>
+      </c>
+      <c r="O13" s="98" cm="1">
+        <f t="array" ref="O13">IF(O12&gt;0,bankers_round(N13+N12*(1-$G$21),2),bankers_round(N13+N12,2))</f>
+        <v>2891.54</v>
+      </c>
+      <c r="P13" s="98" cm="1">
+        <f t="array" ref="P13">IF(P12&gt;0,bankers_round(O13+O12*(1-$G$21),2),bankers_round(O13+O12,2))</f>
+        <v>3354.69</v>
+      </c>
+      <c r="Q13" s="40" cm="1">
+        <f t="array" ref="Q13">IF(Q12&gt;0,bankers_round(P13+P12*(1-$G$21),2),bankers_round(P13+P12,2))</f>
+        <v>3904.66</v>
       </c>
       <c r="U13" s="74"/>
     </row>
@@ -1488,51 +1497,51 @@
       <c r="B14" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="97">
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="99">
         <v>1000</v>
       </c>
-      <c r="H14" s="93">
-        <f>G14*H15</f>
+      <c r="H14" s="95" cm="1">
+        <f t="array" ref="H14">bankers_round(G14*H15, 0)</f>
         <v>1000</v>
       </c>
-      <c r="I14" s="93">
-        <f t="shared" ref="I14:P14" si="1">H14*I15</f>
+      <c r="I14" s="95" cm="1">
+        <f t="array" ref="I14">bankers_round(H14*I15, 0)</f>
         <v>1000</v>
       </c>
-      <c r="J14" s="93">
-        <f t="shared" si="1"/>
+      <c r="J14" s="95" cm="1">
+        <f t="array" ref="J14">bankers_round(I14*J15, 0)</f>
         <v>1000</v>
       </c>
-      <c r="K14" s="93">
-        <f t="shared" si="1"/>
+      <c r="K14" s="95" cm="1">
+        <f t="array" ref="K14">bankers_round(J14*K15, 0)</f>
         <v>1000</v>
       </c>
-      <c r="L14" s="93">
-        <f t="shared" si="1"/>
+      <c r="L14" s="95" cm="1">
+        <f t="array" ref="L14">bankers_round(K14*L15, 0)</f>
         <v>1000</v>
       </c>
-      <c r="M14" s="93">
-        <f t="shared" si="1"/>
+      <c r="M14" s="95" cm="1">
+        <f t="array" ref="M14">bankers_round(L14*M15, 0)</f>
         <v>1000</v>
       </c>
-      <c r="N14" s="93">
-        <f t="shared" si="1"/>
+      <c r="N14" s="95" cm="1">
+        <f t="array" ref="N14">bankers_round(M14*N15, 0)</f>
         <v>1000</v>
       </c>
-      <c r="O14" s="93">
-        <f t="shared" si="1"/>
+      <c r="O14" s="95" cm="1">
+        <f t="array" ref="O14">bankers_round(N14*O15, 0)</f>
         <v>1000</v>
       </c>
-      <c r="P14" s="93">
-        <f t="shared" si="1"/>
+      <c r="P14" s="95" cm="1">
+        <f t="array" ref="P14">bankers_round(O14*P15, 0)</f>
         <v>1000</v>
       </c>
-      <c r="Q14" s="41">
-        <f>P14*P15</f>
+      <c r="Q14" s="41" cm="1">
+        <f t="array" ref="Q14">bankers_round(P14*Q15, 0)</f>
         <v>1000</v>
       </c>
     </row>
@@ -1540,36 +1549,36 @@
       <c r="B15" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="94"/>
-      <c r="G15" s="97"/>
-      <c r="H15" s="90">
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="99"/>
+      <c r="H15" s="93">
         <v>1</v>
       </c>
-      <c r="I15" s="90">
+      <c r="I15" s="93">
         <v>1</v>
       </c>
-      <c r="J15" s="90">
+      <c r="J15" s="93">
         <v>1</v>
       </c>
-      <c r="K15" s="90">
+      <c r="K15" s="93">
         <v>1</v>
       </c>
-      <c r="L15" s="90">
+      <c r="L15" s="93">
         <v>1</v>
       </c>
-      <c r="M15" s="90">
+      <c r="M15" s="93">
         <v>1</v>
       </c>
-      <c r="N15" s="90">
+      <c r="N15" s="93">
         <v>1</v>
       </c>
-      <c r="O15" s="90">
+      <c r="O15" s="93">
         <v>1</v>
       </c>
-      <c r="P15" s="90">
+      <c r="P15" s="93">
         <v>1</v>
       </c>
       <c r="Q15" s="67">
@@ -1580,479 +1589,484 @@
       <c r="B16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="94"/>
-      <c r="G16" s="98">
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="100">
         <v>5</v>
       </c>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
-      <c r="L16" s="75"/>
-      <c r="M16" s="75"/>
-      <c r="N16" s="75"/>
-      <c r="O16" s="75"/>
-      <c r="P16" s="75"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="85"/>
+      <c r="K16" s="85"/>
+      <c r="L16" s="85"/>
+      <c r="M16" s="85"/>
+      <c r="N16" s="85"/>
+      <c r="O16" s="85"/>
+      <c r="P16" s="85"/>
       <c r="Q16" s="21"/>
     </row>
     <row r="17" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="93"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="99">
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="101">
         <v>15</v>
       </c>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="75"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75"/>
-      <c r="O17" s="75"/>
-      <c r="P17" s="75"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="85"/>
+      <c r="J17" s="85"/>
+      <c r="K17" s="85"/>
+      <c r="L17" s="85"/>
+      <c r="M17" s="85"/>
+      <c r="N17" s="85"/>
+      <c r="O17" s="85"/>
+      <c r="P17" s="85"/>
       <c r="Q17" s="21"/>
     </row>
     <row r="18" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="94"/>
-      <c r="G18" s="91">
-        <v>0.22</v>
-      </c>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="84">
+        <v>0.19</v>
+      </c>
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="85"/>
+      <c r="L18" s="85"/>
+      <c r="M18" s="85"/>
+      <c r="N18" s="85"/>
+      <c r="O18" s="85"/>
+      <c r="P18" s="85"/>
       <c r="Q18" s="21"/>
     </row>
     <row r="19" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="91">
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="84">
         <v>0.1</v>
       </c>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="75"/>
-      <c r="O19" s="75"/>
-      <c r="P19" s="75"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="85"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="85"/>
+      <c r="L19" s="85"/>
+      <c r="M19" s="85"/>
+      <c r="N19" s="85"/>
+      <c r="O19" s="85"/>
+      <c r="P19" s="85"/>
       <c r="Q19" s="21"/>
     </row>
     <row r="20" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="71">
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="84">
         <v>0.05</v>
       </c>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="27"/>
-    </row>
-    <row r="22" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="10"/>
-      <c r="D22" s="1"/>
-      <c r="F22" s="6"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="85"/>
+      <c r="L20" s="85"/>
+      <c r="M20" s="85"/>
+      <c r="N20" s="85"/>
+      <c r="O20" s="85"/>
+      <c r="P20" s="85"/>
+      <c r="Q20" s="21"/>
+    </row>
+    <row r="21" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="71">
+        <v>0</v>
+      </c>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="27"/>
     </row>
     <row r="23" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="10"/>
       <c r="D23" s="1"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-    </row>
-    <row r="24" spans="2:17" s="3" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="9"/>
-      <c r="E24" s="5"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-    </row>
-    <row r="25" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="F25" s="6"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-    </row>
-    <row r="26" spans="2:17" s="3" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="42" t="s">
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="10"/>
+      <c r="D24" s="1"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+    </row>
+    <row r="25" spans="2:17" s="3" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="9"/>
+      <c r="E25" s="5"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+    </row>
+    <row r="26" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="F26" s="6"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+    </row>
+    <row r="27" spans="2:17" s="3" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="45"/>
-    </row>
-    <row r="27" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="50">
-        <v>0</v>
-      </c>
-      <c r="H27" s="50">
-        <f>+G27+1</f>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="45"/>
+    </row>
+    <row r="28" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="50">
+        <v>0</v>
+      </c>
+      <c r="H28" s="50">
+        <f>+G28+1</f>
         <v>1</v>
       </c>
-      <c r="I27" s="50">
-        <f t="shared" ref="I27:P27" si="2">+H27+1</f>
+      <c r="I28" s="50">
+        <f t="shared" ref="I28:P28" si="1">+H28+1</f>
         <v>2</v>
       </c>
-      <c r="J27" s="50">
-        <f t="shared" si="2"/>
+      <c r="J28" s="50">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K27" s="50">
-        <f t="shared" si="2"/>
+      <c r="K28" s="50">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L27" s="50">
-        <f t="shared" si="2"/>
+      <c r="L28" s="50">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M27" s="50">
-        <f t="shared" si="2"/>
+      <c r="M28" s="50">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="N27" s="50">
-        <f t="shared" si="2"/>
+      <c r="N28" s="50">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="O27" s="50">
-        <f t="shared" si="2"/>
+      <c r="O28" s="50">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="P27" s="50">
-        <f t="shared" si="2"/>
+      <c r="P28" s="50">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="Q27" s="51" t="s">
+      <c r="Q28" s="51" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="28" t="s">
+    <row r="29" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="77" cm="1">
-        <f t="array" ref="G28">bankers_round($G$16*G14/G12, 2)</f>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="77" cm="1">
+        <f t="array" ref="G29">bankers_round($G$16*G14/G12, 2)</f>
         <v>10</v>
       </c>
-      <c r="H28" s="77" t="e" cm="1">
-        <f t="array" aca="1" ref="H28" ca="1">bankers_round($G$16*H14/H12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I28" s="77" t="e" cm="1">
-        <f t="array" aca="1" ref="I28" ca="1">bankers_round($G$16*I14/I12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J28" s="77" t="e" cm="1">
-        <f t="array" aca="1" ref="J28" ca="1">bankers_round($G$16*J14/J12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K28" s="77" t="e" cm="1">
-        <f t="array" aca="1" ref="K28" ca="1">bankers_round($G$16*K14/K12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L28" s="77" t="e" cm="1">
-        <f t="array" aca="1" ref="L28" ca="1">bankers_round($G$16*L14/L12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M28" s="77" t="e" cm="1">
-        <f t="array" aca="1" ref="M28" ca="1">bankers_round($G$16*M14/M12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N28" s="77" t="e" cm="1">
-        <f t="array" aca="1" ref="N28" ca="1">bankers_round($G$16*N14/N12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="O28" s="77" t="e" cm="1">
-        <f t="array" aca="1" ref="O28" ca="1">bankers_round($G$16*O14/O12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="P28" s="77" t="e" cm="1">
-        <f t="array" aca="1" ref="P28" ca="1">bankers_round($G$16*P14/P12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Q28" s="64" t="e" cm="1">
-        <f t="array" aca="1" ref="Q28" ca="1">bankers_round($G$16*Q14/Q12, 2)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="80" cm="1">
-        <f t="array" ref="G29">bankers_round($G$28*G12/G14, 2)</f>
-        <v>5</v>
-      </c>
-      <c r="H29" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="H29" ca="1">bankers_round($G$28*H12/H14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I29" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="I29" ca="1">bankers_round($G$28*I12/I14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J29" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="J29" ca="1">bankers_round($G$28*J12/J14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K29" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="K29" ca="1">bankers_round($G$28*K12/K14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L29" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="L29" ca="1">bankers_round($G$28*L12/L14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M29" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="M29" ca="1">bankers_round($G$28*M12/M14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N29" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="N29" ca="1">bankers_round($G$28*N12/N14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="O29" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="O29" ca="1">bankers_round($G$28*O12/O14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="P29" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="P29" ca="1">bankers_round($G$28*P12/P14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Q29" s="65" t="e" cm="1">
-        <f t="array" aca="1" ref="Q29" ca="1">bankers_round($G$28*Q12/Q14, 2)</f>
-        <v>#NAME?</v>
+      <c r="H29" s="77" cm="1">
+        <f t="array" ref="H29">bankers_round($G$16*H14/H12, 2)</f>
+        <v>123.46</v>
+      </c>
+      <c r="I29" s="77" cm="1">
+        <f t="array" ref="I29">bankers_round($G$16*I14/I12, 2)</f>
+        <v>58.79</v>
+      </c>
+      <c r="J29" s="77" cm="1">
+        <f t="array" ref="J29">bankers_round($G$16*J14/J12, 2)</f>
+        <v>37.299999999999997</v>
+      </c>
+      <c r="K29" s="77" cm="1">
+        <f t="array" ref="K29">bankers_round($G$16*K14/K12, 2)</f>
+        <v>26.6</v>
+      </c>
+      <c r="L29" s="77" cm="1">
+        <f t="array" ref="L29">bankers_round($G$16*L14/L12, 2)</f>
+        <v>20.22</v>
+      </c>
+      <c r="M29" s="77" cm="1">
+        <f t="array" ref="M29">bankers_round($G$16*M14/M12, 2)</f>
+        <v>16</v>
+      </c>
+      <c r="N29" s="77" cm="1">
+        <f t="array" ref="N29">bankers_round($G$16*N14/N12, 2)</f>
+        <v>13.01</v>
+      </c>
+      <c r="O29" s="77" cm="1">
+        <f t="array" ref="O29">bankers_round($G$16*O14/O12, 2)</f>
+        <v>10.8</v>
+      </c>
+      <c r="P29" s="77" cm="1">
+        <f t="array" ref="P29">bankers_round($G$16*P14/P12, 2)</f>
+        <v>9.09</v>
+      </c>
+      <c r="Q29" s="64" cm="1">
+        <f t="array" ref="Q29">bankers_round($G$16*Q14/Q12, 2)</f>
+        <v>7.75</v>
       </c>
     </row>
     <row r="30" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30" s="78"/>
       <c r="D30" s="78"/>
       <c r="E30" s="79"/>
       <c r="F30" s="78"/>
       <c r="G30" s="80" cm="1">
-        <f t="array" ref="G30">bankers_round($G$17*G12/$G$14, 2)</f>
+        <f t="array" ref="G30">bankers_round($G$29*G12/G14, 2)</f>
+        <v>5</v>
+      </c>
+      <c r="H30" s="80" cm="1">
+        <f t="array" ref="H30">bankers_round($G$29*H12/H14, 2)</f>
+        <v>0.4</v>
+      </c>
+      <c r="I30" s="80" cm="1">
+        <f t="array" ref="I30">bankers_round($G$29*I12/I14, 2)</f>
+        <v>0.85</v>
+      </c>
+      <c r="J30" s="80" cm="1">
+        <f t="array" ref="J30">bankers_round($G$29*J12/J14, 2)</f>
+        <v>1.34</v>
+      </c>
+      <c r="K30" s="80" cm="1">
+        <f t="array" ref="K30">bankers_round($G$29*K12/K14, 2)</f>
+        <v>1.88</v>
+      </c>
+      <c r="L30" s="80" cm="1">
+        <f t="array" ref="L30">bankers_round($G$29*L12/L14, 2)</f>
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="M30" s="80" cm="1">
+        <f t="array" ref="M30">bankers_round($G$29*M12/M14, 2)</f>
+        <v>3.12</v>
+      </c>
+      <c r="N30" s="80" cm="1">
+        <f t="array" ref="N30">bankers_round($G$29*N12/N14, 2)</f>
+        <v>3.84</v>
+      </c>
+      <c r="O30" s="80" cm="1">
+        <f t="array" ref="O30">bankers_round($G$29*O12/O14, 2)</f>
+        <v>4.63</v>
+      </c>
+      <c r="P30" s="80" cm="1">
+        <f t="array" ref="P30">bankers_round($G$29*P12/P14, 2)</f>
+        <v>5.5</v>
+      </c>
+      <c r="Q30" s="65" cm="1">
+        <f t="array" ref="Q30">bankers_round($G$29*Q12/Q14, 2)</f>
+        <v>6.45</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="78"/>
+      <c r="G31" s="80" cm="1">
+        <f t="array" ref="G31">bankers_round($G$17*G12/$G$14, 2)</f>
         <v>7.5</v>
       </c>
-      <c r="H30" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="H30" ca="1">bankers_round($G$17*H12/$G$14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I30" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="I30" ca="1">bankers_round($G$17*I12/$G$14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J30" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="J30" ca="1">bankers_round($G$17*J12/$G$14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K30" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="K30" ca="1">bankers_round($G$17*K12/$G$14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L30" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="L30" ca="1">bankers_round($G$17*L12/$G$14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M30" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="M30" ca="1">bankers_round($G$17*M12/$G$14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N30" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="N30" ca="1">bankers_round($G$17*N12/$G$14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="O30" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="O30" ca="1">bankers_round($G$17*O12/$G$14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="P30" s="80" t="e" cm="1">
-        <f t="array" aca="1" ref="P30" ca="1">bankers_round($G$17*P12/$G$14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Q30" s="65" t="e" cm="1">
-        <f t="array" aca="1" ref="Q30" ca="1">bankers_round($G$17*Q12/$G$14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="30" t="s">
+      <c r="H31" s="80" cm="1">
+        <f t="array" ref="H31">bankers_round($G$17*H12/$G$14, 2)</f>
+        <v>0.61</v>
+      </c>
+      <c r="I31" s="80" cm="1">
+        <f t="array" ref="I31">bankers_round($G$17*I12/$G$14, 2)</f>
+        <v>1.28</v>
+      </c>
+      <c r="J31" s="80" cm="1">
+        <f t="array" ref="J31">bankers_round($G$17*J12/$G$14, 2)</f>
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="K31" s="80" cm="1">
+        <f t="array" ref="K31">bankers_round($G$17*K12/$G$14, 2)</f>
+        <v>2.82</v>
+      </c>
+      <c r="L31" s="80" cm="1">
+        <f t="array" ref="L31">bankers_round($G$17*L12/$G$14, 2)</f>
+        <v>3.71</v>
+      </c>
+      <c r="M31" s="80" cm="1">
+        <f t="array" ref="M31">bankers_round($G$17*M12/$G$14, 2)</f>
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="N31" s="80" cm="1">
+        <f t="array" ref="N31">bankers_round($G$17*N12/$G$14, 2)</f>
+        <v>5.76</v>
+      </c>
+      <c r="O31" s="80" cm="1">
+        <f t="array" ref="O31">bankers_round($G$17*O12/$G$14, 2)</f>
+        <v>6.95</v>
+      </c>
+      <c r="P31" s="80" cm="1">
+        <f t="array" ref="P31">bankers_round($G$17*P12/$G$14, 2)</f>
+        <v>8.25</v>
+      </c>
+      <c r="Q31" s="65" cm="1">
+        <f t="array" ref="Q31">bankers_round($G$17*Q12/$G$14, 2)</f>
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="33" t="e" cm="1">
-        <f t="array" aca="1" ref="G31" ca="1">bankers_round((G13+(H12-G13*G19)/(1+G19)^1+(I12-H13*G19)/(1+G19)^2+(J12-I13*G19)/(1+G19)^3+(K12-J13*G19)/(1+G19)^4+(L12-K13*G19)/(1+G19)^5+(M12-L13*G19)/(1+G19)^6+(N12-M13*G19)/(1+G19)^7+(O12-N13*G19)/(1+G19)^8+(P12-O13*G19)/(1+G19)^9+(Q12-P13*G19)/(1+G19)^10+((Q12-P13*G19)/(G19-G20))/(1+G19)^10)/G14, 2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H31" s="66"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="66"/>
-      <c r="K31" s="66"/>
-      <c r="L31" s="66"/>
-      <c r="M31" s="66"/>
-      <c r="N31" s="66"/>
-      <c r="O31" s="34"/>
-      <c r="P31" s="34"/>
-      <c r="Q31" s="27"/>
-    </row>
-    <row r="32" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="13"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-    </row>
-    <row r="33" spans="1:16" s="3" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="15"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="33" cm="1">
+        <f t="array" ref="G32">bankers_round((G13+(H12-G13*G19)/(1+G19)^1+(I12-H13*G19)/(1+G19)^2+(J12-I13*G19)/(1+G19)^3+(K12-J13*G19)/(1+G19)^4+(L12-K13*G19)/(1+G19)^5+(M12-L13*G19)/(1+G19)^6+(N12-M13*G19)/(1+G19)^7+(O12-N13*G19)/(1+G19)^8+(P12-O13*G19)/(1+G19)^9+(Q12-P13*G19)/(1+G19)^10+((Q12-P13*G19)/(G19-G21))/(1+G19)^10)/G14, 2)</f>
+        <v>2.61</v>
+      </c>
+      <c r="H32" s="66"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="66"/>
+      <c r="L32" s="66"/>
+      <c r="M32" s="66"/>
+      <c r="N32" s="66"/>
+      <c r="O32" s="34"/>
+      <c r="P32" s="34"/>
+      <c r="Q32" s="27"/>
+    </row>
+    <row r="33" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="13"/>
       <c r="M33" s="2"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-    </row>
-    <row r="34" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="1:16" s="3" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="15"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-    </row>
-    <row r="35" spans="1:16" s="3" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="5"/>
+      <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
-    </row>
-    <row r="36" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+    </row>
+    <row r="36" spans="1:16" s="3" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G36" s="2"/>
+      <c r="H36" s="5"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
     </row>
     <row r="37" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="16"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="G37" s="11"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -2066,9 +2080,10 @@
     <row r="38" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="G38" s="11"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="16"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -2096,12 +2111,11 @@
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="12"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="G40" s="11"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -2113,10 +2127,12 @@
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="1"/>
-      <c r="D41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="12"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -2128,12 +2144,10 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="15"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -2145,11 +2159,12 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="15"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -2308,11 +2323,27 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
     </row>
     <row r="54" spans="2:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="2:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>